<commit_message>
Edited Result Table Fonts
</commit_message>
<xml_diff>
--- a/Final Model Test Results Summary.xlsx
+++ b/Final Model Test Results Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farhan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CC8088-307F-47CF-932D-A352677F29CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F677ED-1787-4E98-BD37-02E967D3642E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" tabRatio="778" activeTab="4" xr2:uid="{0E0C5392-611A-44B4-A62C-8DB27F347549}"/>
   </bookViews>
@@ -19,6 +19,9 @@
     <sheet name="Pivot - Accuracies" sheetId="8" r:id="rId4"/>
     <sheet name="Results" sheetId="10" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Results!$A$1:$L$21</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId6"/>
@@ -3188,7 +3191,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3211,6 +3214,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3220,7 +3236,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -3516,12 +3532,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="double">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -3619,9 +3693,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3634,8 +3705,106 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -26914,21 +27083,21 @@
         <v>11</v>
       </c>
       <c r="M4" s="7"/>
-      <c r="N4" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="R4" s="41"/>
-      <c r="S4" s="41"/>
-      <c r="T4" s="41" t="s">
+      <c r="N4" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="U4" s="41"/>
-      <c r="V4" s="41"/>
+      <c r="U4" s="45"/>
+      <c r="V4" s="45"/>
       <c r="W4" s="27"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -27452,21 +27621,21 @@
         <v>1044</v>
       </c>
       <c r="N3" s="7"/>
-      <c r="O3" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
-      <c r="U3" s="41" t="s">
+      <c r="O3" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" s="45"/>
+      <c r="T3" s="45"/>
+      <c r="U3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="V3" s="41"/>
-      <c r="W3" s="41"/>
+      <c r="V3" s="45"/>
+      <c r="W3" s="45"/>
     </row>
     <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -27579,7 +27748,7 @@
       <c r="V5" s="15">
         <v>0.8</v>
       </c>
-      <c r="W5" s="42">
+      <c r="W5" s="41">
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -27644,7 +27813,7 @@
       <c r="V6" s="17">
         <v>0.9285714285714286</v>
       </c>
-      <c r="W6" s="43">
+      <c r="W6" s="42">
         <v>0.92307692307692313</v>
       </c>
     </row>
@@ -27709,7 +27878,7 @@
       <c r="V7" s="17">
         <v>0.75</v>
       </c>
-      <c r="W7" s="43">
+      <c r="W7" s="42">
         <v>0.72727272727272729</v>
       </c>
     </row>
@@ -27774,7 +27943,7 @@
       <c r="V8" s="17">
         <v>0.6</v>
       </c>
-      <c r="W8" s="43">
+      <c r="W8" s="42">
         <v>0.75</v>
       </c>
     </row>
@@ -27839,7 +28008,7 @@
       <c r="V9" s="20">
         <v>1</v>
       </c>
-      <c r="W9" s="44">
+      <c r="W9" s="43">
         <v>1</v>
       </c>
     </row>
@@ -27904,7 +28073,7 @@
       <c r="V10" s="30">
         <v>0.84782608695652173</v>
       </c>
-      <c r="W10" s="45">
+      <c r="W10" s="44">
         <v>0.8666666666666667</v>
       </c>
     </row>
@@ -28668,530 +28837,542 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4498395-F7A9-4014-952B-D111D794B7F9}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:L21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="47"/>
+    <col min="2" max="2" width="14.21875" style="47" customWidth="1"/>
+    <col min="3" max="4" width="7.21875" style="47" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" style="47" customWidth="1"/>
+    <col min="6" max="7" width="7.21875" style="47" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" style="47" customWidth="1"/>
+    <col min="9" max="10" width="7.21875" style="47" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" style="47" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="46" t="s">
         <v>1048</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="7"/>
-      <c r="C3" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41" t="s">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="48"/>
+      <c r="C3" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="27"/>
-    </row>
-    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="5" t="s">
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="50"/>
+    </row>
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="13" t="s">
+      <c r="C4" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="F4" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="13" t="s">
+      <c r="I4" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="28" t="s">
+      <c r="L4" s="53" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="55">
         <v>0.05</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="56">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="78">
         <v>9.4E-2</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="55">
         <v>1.2E-2</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="56">
         <v>1.2E-2</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="78">
         <v>2.4E-2</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="55">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="56">
         <v>0.02</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="78">
         <v>2.4E-2</v>
       </c>
-      <c r="L5" s="23">
+      <c r="L5" s="58">
         <v>0.14199999999999999</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="55">
         <v>0.108</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="60">
         <v>0.114</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="79">
         <v>0.222</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="55">
         <v>1.6E-2</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="60">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="79">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="55">
         <v>2.4E-2</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="60">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="79">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="L6" s="24">
+      <c r="L6" s="62">
         <v>0.308</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="55">
         <v>0.09</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="60">
         <v>0.106</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="79">
         <v>0.19600000000000001</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="55">
         <v>0.03</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="60">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="79">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="55">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="60">
         <v>1.6E-2</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="79">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="L7" s="24">
+      <c r="L7" s="62">
         <v>0.27</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="55">
         <v>0.03</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="60">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="79">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="55">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="60">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="79">
         <v>0.01</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="55">
         <v>1.4E-2</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="60">
         <v>0.01</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="79">
         <v>2.4E-2</v>
       </c>
-      <c r="L8" s="24">
+      <c r="L8" s="62">
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="11" t="s">
+    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="64">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="65">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="80">
         <v>0.124</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="64">
         <v>1.2E-2</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="65">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="80">
         <v>0.03</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="64">
         <v>0.01</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="65">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="K9" s="21">
+      <c r="K9" s="80">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9" s="67">
         <v>0.182</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="16.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="12" t="s">
+    <row r="10" spans="2:12" ht="16.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="69">
         <v>0.34399999999999997</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="70">
         <v>0.35599999999999998</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="81">
         <v>0.7</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="69">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="70">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="81">
         <v>0.15</v>
       </c>
-      <c r="I10" s="29">
+      <c r="I10" s="69">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="J10" s="30">
+      <c r="J10" s="70">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="K10" s="22">
+      <c r="K10" s="81">
         <v>0.15</v>
       </c>
-      <c r="L10" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="46" t="s">
+      <c r="L10" s="72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="73" t="s">
         <v>1046</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
-      <c r="C14" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41" t="s">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="48"/>
+      <c r="C14" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-    </row>
-    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="5" t="s">
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+    </row>
+    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="13" t="s">
+      <c r="C15" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="52" t="s">
         <v>1044</v>
       </c>
-      <c r="F15" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" s="13" t="s">
+      <c r="F15" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="52" t="s">
         <v>1044</v>
       </c>
-      <c r="I15" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="13" t="s">
+      <c r="I15" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="52" t="s">
         <v>1044</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="9" t="s">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="55">
         <v>0.88</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="56">
         <v>0.77272727272727271</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="57">
         <v>0.82978723404255317</v>
       </c>
-      <c r="F16" s="14">
-        <v>1</v>
-      </c>
-      <c r="G16" s="15">
+      <c r="F16" s="55">
+        <v>1</v>
+      </c>
+      <c r="G16" s="56">
         <v>0.83333333333333337</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="57">
         <v>0.91666666666666663</v>
       </c>
-      <c r="I16" s="14">
-        <v>1</v>
-      </c>
-      <c r="J16" s="15">
+      <c r="I16" s="55">
+        <v>1</v>
+      </c>
+      <c r="J16" s="56">
         <v>0.8</v>
       </c>
-      <c r="K16" s="42">
+      <c r="K16" s="74">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="55">
         <v>0.92592592592592593</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="60">
         <v>0.80701754385964908</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="61">
         <v>0.86486486486486491</v>
       </c>
-      <c r="F17" s="14">
-        <v>1</v>
-      </c>
-      <c r="G17" s="17">
+      <c r="F17" s="55">
+        <v>1</v>
+      </c>
+      <c r="G17" s="60">
         <v>0.55555555555555558</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="61">
         <v>0.76470588235294112</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="55">
         <v>0.91666666666666663</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J17" s="60">
         <v>0.9285714285714286</v>
       </c>
-      <c r="K17" s="43">
+      <c r="K17" s="75">
         <v>0.92307692307692313</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B18" s="10" t="s">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="55">
         <v>0.91111111111111109</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="60">
         <v>0.81132075471698117</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="61">
         <v>0.8571428571428571</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="55">
         <v>0.73333333333333328</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="60">
         <v>0.81818181818181823</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="61">
         <v>0.76923076923076927</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="55">
         <v>0.66666666666666663</v>
       </c>
-      <c r="J18" s="17">
+      <c r="J18" s="60">
         <v>0.75</v>
       </c>
-      <c r="K18" s="43">
+      <c r="K18" s="75">
         <v>0.72727272727272729</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="10" t="s">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="55">
         <v>0.8666666666666667</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="60">
         <v>0.70588235294117652</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="61">
         <v>0.78125</v>
       </c>
-      <c r="F19" s="14">
-        <v>1</v>
-      </c>
-      <c r="G19" s="17">
-        <v>1</v>
-      </c>
-      <c r="H19" s="18">
-        <v>1</v>
-      </c>
-      <c r="I19" s="14">
+      <c r="F19" s="55">
+        <v>1</v>
+      </c>
+      <c r="G19" s="60">
+        <v>1</v>
+      </c>
+      <c r="H19" s="61">
+        <v>1</v>
+      </c>
+      <c r="I19" s="55">
         <v>0.8571428571428571</v>
       </c>
-      <c r="J19" s="17">
+      <c r="J19" s="60">
         <v>0.6</v>
       </c>
-      <c r="K19" s="43">
+      <c r="K19" s="75">
         <v>0.75</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="11" t="s">
+    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="64">
         <v>0.90909090909090906</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="65">
         <v>0.86206896551724133</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="66">
         <v>0.88709677419354838</v>
       </c>
-      <c r="F20" s="19">
-        <v>1</v>
-      </c>
-      <c r="G20" s="20">
+      <c r="F20" s="64">
+        <v>1</v>
+      </c>
+      <c r="G20" s="65">
         <v>0.77777777777777779</v>
       </c>
-      <c r="H20" s="21">
+      <c r="H20" s="66">
         <v>0.88709677419354838</v>
       </c>
-      <c r="I20" s="19">
-        <v>1</v>
-      </c>
-      <c r="J20" s="20">
-        <v>1</v>
-      </c>
-      <c r="K20" s="44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" ht="16.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="12" t="s">
+      <c r="I20" s="64">
+        <v>1</v>
+      </c>
+      <c r="J20" s="65">
+        <v>1</v>
+      </c>
+      <c r="K20" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="16.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="68" t="s">
         <v>1045</v>
       </c>
-      <c r="C21" s="29">
+      <c r="C21" s="69">
         <v>0.90697674418604646</v>
       </c>
-      <c r="D21" s="30">
+      <c r="D21" s="70">
         <v>0.8033707865168539</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="71">
         <v>0.85428571428571431</v>
       </c>
-      <c r="F21" s="29">
+      <c r="F21" s="69">
         <v>0.89473684210526316</v>
       </c>
-      <c r="G21" s="30">
+      <c r="G21" s="70">
         <v>0.7567567567567568</v>
       </c>
-      <c r="H21" s="22">
+      <c r="H21" s="71">
         <v>0.82666666666666666</v>
       </c>
-      <c r="I21" s="29">
+      <c r="I21" s="69">
         <v>0.89655172413793105</v>
       </c>
-      <c r="J21" s="30">
+      <c r="J21" s="70">
         <v>0.84782608695652173</v>
       </c>
-      <c r="K21" s="45">
+      <c r="K21" s="77">
         <v>0.8666666666666667</v>
       </c>
     </row>
@@ -29205,5 +29386,6 @@
     <mergeCell ref="I14:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>